<commit_message>
requirements added, ontology starting to ve clean
</commit_message>
<xml_diff>
--- a/ontology/requirements/requirements.xlsx
+++ b/ontology/requirements/requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/SPEECH/ontology/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4515EF-73E2-5C41-A47A-45C0E09B97AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B9BA77-5CE7-8148-9CE9-599072F8CD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28880" yWindow="1100" windowWidth="11700" windowHeight="17500" xr2:uid="{E3B92CCF-2AD2-9D49-BEEA-2419F5A8B9FD}"/>
+    <workbookView xWindow="28920" yWindow="-840" windowWidth="19640" windowHeight="21100" xr2:uid="{E3B92CCF-2AD2-9D49-BEEA-2419F5A8B9FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Identifier</t>
   </si>
@@ -65,12 +65,6 @@
     <t>An speech has an ideology associated</t>
   </si>
   <si>
-    <t>An election period can be identified</t>
-  </si>
-  <si>
-    <t>A political party can be identified</t>
-  </si>
-  <si>
     <t>The political parties have accounts in social networks associated</t>
   </si>
   <si>
@@ -80,24 +74,9 @@
     <t>A political party may have political manifestos</t>
   </si>
   <si>
-    <t>A political party may have a hashtag associated to a political campaign</t>
-  </si>
-  <si>
-    <t>The comunication channels may have interactions</t>
-  </si>
-  <si>
-    <t>An speech may have metrics</t>
-  </si>
-  <si>
     <t>speech-r4</t>
   </si>
   <si>
-    <t>speech-r5</t>
-  </si>
-  <si>
-    <t>speech-r6</t>
-  </si>
-  <si>
     <t>speech-r7</t>
   </si>
   <si>
@@ -110,9 +89,6 @@
     <t>speech-r10</t>
   </si>
   <si>
-    <t>speech-r11</t>
-  </si>
-  <si>
     <t>speech-r12</t>
   </si>
   <si>
@@ -170,16 +146,55 @@
     <t>An speech has a subject associated</t>
   </si>
   <si>
-    <t>consulta sparql adicional para likear a wikidata</t>
-  </si>
-  <si>
-    <t>lista de todos partidos politicos</t>
-  </si>
-  <si>
-    <t>manifiesto no incluye interacción, de twits: citar, rt, responder concita, responder, like, ...</t>
-  </si>
-  <si>
-    <t>esto son las interactions counter; schema modela los tipos de interacción</t>
+    <t>A political party may have a hashtag associated to a speech</t>
+  </si>
+  <si>
+    <t>An speech may have interaction metrics</t>
+  </si>
+  <si>
+    <t>Which are the threads previous to the 2021 elections in Madrid of all parties?</t>
+  </si>
+  <si>
+    <t>que hilo de qué?</t>
+  </si>
+  <si>
+    <t>Which is the previous tweet of the elections of Madrid in 2015?</t>
+  </si>
+  <si>
+    <t>Which is the user most mentioned by a political party?</t>
+  </si>
+  <si>
+    <t>Which is the user most cited by a political party?</t>
+  </si>
+  <si>
+    <t>Which is the tweet with more citations of a political party?</t>
+  </si>
+  <si>
+    <t>Which are the tweets and users cited by at least two political parties?</t>
+  </si>
+  <si>
+    <t>Which are the tweets and users retweeted by at least two political parties?</t>
+  </si>
+  <si>
+    <t>Which is the most cited or retweeted tweet by the more number of political parties?</t>
+  </si>
+  <si>
+    <t>Which is the tweet of a political party most retweeted by another political party?</t>
+  </si>
+  <si>
+    <t>Which is the hashtag most tweeted by a political party in the 2019 Madrid elections?</t>
+  </si>
+  <si>
+    <t>Which is the most wetweeted hashtag by a political party in the 2019 Madrid elections?</t>
+  </si>
+  <si>
+    <t>Which is the political party that has tweeted the most in 2021?</t>
+  </si>
+  <si>
+    <t>Which is the political party that has been retweeted the most in 2021?</t>
+  </si>
+  <si>
+    <t>How have ODS changed in the proposals of a manifesto of a political party?</t>
   </si>
 </sst>
 </file>
@@ -245,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -254,6 +269,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -570,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD387039-14E8-1C40-88EB-6D939C392012}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,174 +632,183 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B19" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B20" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B21" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B23" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B24" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>40</v>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>